<commit_message>
Balanced most of the characters. Everything is much better.
</commit_message>
<xml_diff>
--- a/Character Hit Speeds.xlsx
+++ b/Character Hit Speeds.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avery\Projects\AgeofAnime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{289E3927-5F0B-4616-82AF-943EF52F34EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A06BA36-AAD6-4CB1-8034-C142E586E7B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{024B0EBD-C732-470B-A7BD-B87DD965A47F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Kakashi</t>
   </si>
@@ -104,19 +104,22 @@
     <t>2.0 +- .2</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>=</t>
-  </si>
-  <si>
-    <t>/</t>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Damage per Second</t>
+  </si>
+  <si>
+    <t>Range Damage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -154,11 +157,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -173,9 +173,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD0DA8B3-F9BD-405B-9EDD-F3DE13204641}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,27 +503,42 @@
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="9"/>
       <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -536,13 +553,20 @@
         <f>D2</f>
         <v>10</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <f>B2/D2</f>
         <v>1.6</v>
       </c>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G2" s="2"/>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2" s="11">
+        <f>H2/F2</f>
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -559,16 +583,30 @@
         <f t="shared" ref="E3:E11" si="0">D3</f>
         <v>8</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <f t="shared" ref="F3:F16" si="1">B3/D3</f>
         <v>1</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <f t="shared" ref="G3:G16" si="2">C3/E3</f>
         <v>1.75</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>12</v>
+      </c>
+      <c r="I3" s="11">
+        <f>H3/F3</f>
+        <v>12</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3" s="10">
+        <f t="shared" ref="K3:K16" si="3">J3/G3</f>
+        <v>5.7142857142857144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -585,16 +623,30 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <f t="shared" si="2"/>
         <v>1.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>50</v>
+      </c>
+      <c r="I4" s="11">
+        <f>H4/F4</f>
+        <v>35.714285714285715</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4" s="10">
+        <f t="shared" si="3"/>
+        <v>5.2631578947368425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -609,13 +661,21 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G5" s="2"/>
+      <c r="H5">
+        <v>45</v>
+      </c>
+      <c r="I5" s="11">
+        <f>H5/F5</f>
+        <v>28.125</v>
+      </c>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -632,17 +692,31 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <f t="shared" si="2"/>
         <v>2.125</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="H6">
+        <v>25</v>
+      </c>
+      <c r="I6" s="11">
+        <f>H6/F6</f>
+        <v>20</v>
+      </c>
+      <c r="J6">
+        <v>11</v>
+      </c>
+      <c r="K6" s="10">
+        <f t="shared" si="3"/>
+        <v>5.1764705882352944</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
@@ -654,35 +728,34 @@
       <c r="D7" s="1">
         <v>10</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>14</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <f t="shared" si="2"/>
         <v>2.2142857142857144</v>
       </c>
       <c r="H7">
-        <v>36</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="11">
+        <f>H7/F7</f>
+        <v>50</v>
+      </c>
+      <c r="J7" s="8">
+        <v>11</v>
+      </c>
+      <c r="K7" s="10">
+        <f t="shared" si="3"/>
+        <v>4.967741935483871</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1">
@@ -696,18 +769,22 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="L8">
-        <f>H7/L7</f>
-        <v>16.363636363636363</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8">
+        <v>80</v>
+      </c>
+      <c r="I8" s="11">
+        <f>H8/F8</f>
+        <v>100</v>
+      </c>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1">
@@ -722,17 +799,31 @@
       <c r="E9" s="1">
         <v>7</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <f t="shared" si="2"/>
         <v>1.7142857142857142</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="H9">
+        <v>60</v>
+      </c>
+      <c r="I9" s="11">
+        <f>H9/F9</f>
+        <v>75</v>
+      </c>
+      <c r="J9">
+        <v>50</v>
+      </c>
+      <c r="K9" s="10">
+        <f t="shared" si="3"/>
+        <v>29.166666666666668</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1">
@@ -747,17 +838,31 @@
       <c r="E10" s="1">
         <v>7</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <f t="shared" si="1"/>
         <v>0.7142857142857143</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="H10">
+        <v>90</v>
+      </c>
+      <c r="I10" s="11">
+        <f>H10/F10</f>
+        <v>126</v>
+      </c>
+      <c r="J10">
+        <v>50</v>
+      </c>
+      <c r="K10" s="10">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1">
@@ -771,17 +876,25 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="G11" s="2"/>
+      <c r="H11">
+        <v>150</v>
+      </c>
+      <c r="I11" s="11">
+        <f>H11/F11</f>
+        <v>120</v>
+      </c>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>6</v>
       </c>
       <c r="C12" s="1">
@@ -793,17 +906,31 @@
       <c r="E12" s="1">
         <v>8</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <f t="shared" si="2"/>
         <v>1.625</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="H12">
+        <v>100</v>
+      </c>
+      <c r="I12" s="11">
+        <f>H12/F12</f>
+        <v>100</v>
+      </c>
+      <c r="J12">
+        <v>100</v>
+      </c>
+      <c r="K12" s="10">
+        <f t="shared" si="3"/>
+        <v>61.53846153846154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="1">
@@ -818,17 +945,31 @@
       <c r="E13" s="1">
         <v>15</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <f t="shared" si="2"/>
         <v>2.4</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="H13">
+        <v>240</v>
+      </c>
+      <c r="I13" s="11">
+        <f>H13/F13</f>
+        <v>160</v>
+      </c>
+      <c r="J13">
+        <v>200</v>
+      </c>
+      <c r="K13" s="10">
+        <f t="shared" si="3"/>
+        <v>83.333333333333343</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1">
@@ -839,17 +980,25 @@
         <v>8</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" ref="E14" si="3">D14</f>
+        <f t="shared" ref="E14" si="4">D14</f>
         <v>8</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <f t="shared" si="1"/>
         <v>1.125</v>
       </c>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="G14" s="2"/>
+      <c r="H14">
+        <v>200</v>
+      </c>
+      <c r="I14" s="11">
+        <f>H14/F14</f>
+        <v>177.77777777777777</v>
+      </c>
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="1">
@@ -864,20 +1013,34 @@
       <c r="E15" s="1">
         <v>10</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="2">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="H15">
+        <v>150</v>
+      </c>
+      <c r="I15" s="11">
+        <f>H15/F15</f>
+        <v>107.14285714285715</v>
+      </c>
+      <c r="J15">
+        <v>150</v>
+      </c>
+      <c r="K15" s="10">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>6</v>
       </c>
       <c r="C16" s="1">
@@ -887,19 +1050,33 @@
         <v>10</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" ref="E16" si="4">D16</f>
-        <v>10</v>
-      </c>
-      <c r="F16" s="6">
+        <f t="shared" ref="E16" si="5">D16</f>
+        <v>10</v>
+      </c>
+      <c r="F16" s="5">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
         <f t="shared" si="2"/>
         <v>1.3</v>
       </c>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>125</v>
+      </c>
+      <c r="I16" s="11">
+        <f>H16/F16</f>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="J16">
+        <v>75</v>
+      </c>
+      <c r="K16" s="10">
+        <f t="shared" si="3"/>
+        <v>57.692307692307693</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>20</v>
       </c>
@@ -908,6 +1085,79 @@
       </c>
       <c r="G18" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="H18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="30" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="31" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -915,7 +1165,7 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F16">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -927,7 +1177,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G16">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -938,6 +1188,30 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I16">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K16">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reworked Pain 's Range Attack
</commit_message>
<xml_diff>
--- a/Character Hit Speeds.xlsx
+++ b/Character Hit Speeds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avery\Projects\AgeofAnime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A06BA36-AAD6-4CB1-8034-C142E586E7B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342AAAE4-28D7-4A3C-A04F-AF814A73FDA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{024B0EBD-C732-470B-A7BD-B87DD965A47F}"/>
   </bookViews>
@@ -173,11 +173,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,7 +495,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,10 +515,10 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="9"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
@@ -561,8 +561,8 @@
       <c r="H2">
         <v>30</v>
       </c>
-      <c r="I2" s="11">
-        <f>H2/F2</f>
+      <c r="I2" s="10">
+        <f t="shared" ref="I2:I16" si="0">H2/F2</f>
         <v>18.75</v>
       </c>
     </row>
@@ -580,29 +580,29 @@
         <v>8</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E11" si="0">D3</f>
+        <f t="shared" ref="E3:E11" si="1">D3</f>
         <v>8</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F16" si="1">B3/D3</f>
+        <f t="shared" ref="F3:F16" si="2">B3/D3</f>
         <v>1</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G16" si="2">C3/E3</f>
+        <f t="shared" ref="G3:G16" si="3">C3/E3</f>
         <v>1.75</v>
       </c>
       <c r="H3">
         <v>12</v>
       </c>
-      <c r="I3" s="11">
-        <f>H3/F3</f>
+      <c r="I3" s="10">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="J3">
         <v>10</v>
       </c>
-      <c r="K3" s="10">
-        <f t="shared" ref="K3:K16" si="3">J3/G3</f>
+      <c r="K3" s="9">
+        <f t="shared" ref="K3:K16" si="4">J3/G3</f>
         <v>5.7142857142857144</v>
       </c>
     </row>
@@ -620,29 +620,29 @@
         <v>10</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.9</v>
       </c>
       <c r="H4">
         <v>50</v>
       </c>
-      <c r="I4" s="11">
-        <f>H4/F4</f>
+      <c r="I4" s="10">
+        <f t="shared" si="0"/>
         <v>35.714285714285715</v>
       </c>
       <c r="J4">
         <v>10</v>
       </c>
-      <c r="K4" s="10">
-        <f t="shared" si="3"/>
+      <c r="K4" s="9">
+        <f t="shared" si="4"/>
         <v>5.2631578947368425</v>
       </c>
     </row>
@@ -658,22 +658,22 @@
         <v>15</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5">
         <v>45</v>
       </c>
-      <c r="I5" s="11">
-        <f>H5/F5</f>
+      <c r="I5" s="10">
+        <f t="shared" si="0"/>
         <v>28.125</v>
       </c>
-      <c r="K5" s="10"/>
+      <c r="K5" s="9"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -683,36 +683,36 @@
         <v>10</v>
       </c>
       <c r="C6" s="1">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1">
         <v>8</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.25</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="2"/>
-        <v>2.125</v>
+        <f t="shared" si="3"/>
+        <v>2.5</v>
       </c>
       <c r="H6">
         <v>25</v>
       </c>
-      <c r="I6" s="11">
-        <f>H6/F6</f>
+      <c r="I6" s="10">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="J6">
         <v>11</v>
       </c>
-      <c r="K6" s="10">
-        <f t="shared" si="3"/>
-        <v>5.1764705882352944</v>
+      <c r="K6" s="9">
+        <f t="shared" si="4"/>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -732,25 +732,25 @@
         <v>14</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.2142857142857144</v>
       </c>
       <c r="H7">
         <v>75</v>
       </c>
-      <c r="I7" s="11">
-        <f>H7/F7</f>
+      <c r="I7" s="10">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="J7" s="8">
         <v>11</v>
       </c>
-      <c r="K7" s="10">
-        <f t="shared" si="3"/>
+      <c r="K7" s="9">
+        <f t="shared" si="4"/>
         <v>4.967741935483871</v>
       </c>
     </row>
@@ -766,22 +766,22 @@
         <v>5</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8">
         <v>80</v>
       </c>
-      <c r="I8" s="11">
-        <f>H8/F8</f>
+      <c r="I8" s="10">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="K8" s="10"/>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -800,25 +800,25 @@
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.7142857142857142</v>
       </c>
       <c r="H9">
         <v>60</v>
       </c>
-      <c r="I9" s="11">
-        <f>H9/F9</f>
+      <c r="I9" s="10">
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="J9">
         <v>50</v>
       </c>
-      <c r="K9" s="10">
-        <f t="shared" si="3"/>
+      <c r="K9" s="9">
+        <f t="shared" si="4"/>
         <v>29.166666666666668</v>
       </c>
     </row>
@@ -839,25 +839,25 @@
         <v>7</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H10">
         <v>90</v>
       </c>
-      <c r="I10" s="11">
-        <f>H10/F10</f>
+      <c r="I10" s="10">
+        <f t="shared" si="0"/>
         <v>126</v>
       </c>
       <c r="J10">
         <v>50</v>
       </c>
-      <c r="K10" s="10">
-        <f t="shared" si="3"/>
+      <c r="K10" s="9">
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
     </row>
@@ -873,22 +873,22 @@
         <v>8</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.25</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11">
         <v>150</v>
       </c>
-      <c r="I11" s="11">
-        <f>H11/F11</f>
+      <c r="I11" s="10">
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="K11" s="10"/>
+      <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -907,25 +907,25 @@
         <v>8</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.625</v>
       </c>
       <c r="H12">
         <v>100</v>
       </c>
-      <c r="I12" s="11">
-        <f>H12/F12</f>
+      <c r="I12" s="10">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J12">
         <v>100</v>
       </c>
-      <c r="K12" s="10">
-        <f t="shared" si="3"/>
+      <c r="K12" s="9">
+        <f t="shared" si="4"/>
         <v>61.53846153846154</v>
       </c>
     </row>
@@ -946,25 +946,25 @@
         <v>15</v>
       </c>
       <c r="F13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.4</v>
       </c>
       <c r="H13">
         <v>240</v>
       </c>
-      <c r="I13" s="11">
-        <f>H13/F13</f>
+      <c r="I13" s="10">
+        <f t="shared" si="0"/>
         <v>160</v>
       </c>
       <c r="J13">
         <v>200</v>
       </c>
-      <c r="K13" s="10">
-        <f t="shared" si="3"/>
+      <c r="K13" s="9">
+        <f t="shared" si="4"/>
         <v>83.333333333333343</v>
       </c>
     </row>
@@ -980,22 +980,22 @@
         <v>8</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" ref="E14" si="4">D14</f>
+        <f t="shared" ref="E14" si="5">D14</f>
         <v>8</v>
       </c>
       <c r="F14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.125</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14">
         <v>200</v>
       </c>
-      <c r="I14" s="11">
-        <f>H14/F14</f>
+      <c r="I14" s="10">
+        <f t="shared" si="0"/>
         <v>177.77777777777777</v>
       </c>
-      <c r="K14" s="10"/>
+      <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
@@ -1014,25 +1014,25 @@
         <v>10</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="H15">
         <v>150</v>
       </c>
-      <c r="I15" s="11">
-        <f>H15/F15</f>
+      <c r="I15" s="10">
+        <f t="shared" si="0"/>
         <v>107.14285714285715</v>
       </c>
       <c r="J15">
         <v>150</v>
       </c>
-      <c r="K15" s="10">
-        <f t="shared" si="3"/>
+      <c r="K15" s="9">
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
     </row>
@@ -1050,29 +1050,29 @@
         <v>10</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" ref="E16" si="5">D16</f>
+        <f t="shared" ref="E16" si="6">D16</f>
         <v>10</v>
       </c>
       <c r="F16" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3</v>
       </c>
       <c r="H16">
         <v>125</v>
       </c>
-      <c r="I16" s="11">
-        <f>H16/F16</f>
+      <c r="I16" s="10">
+        <f t="shared" si="0"/>
         <v>208.33333333333334</v>
       </c>
       <c r="J16">
         <v>75</v>
       </c>
-      <c r="K16" s="10">
-        <f t="shared" si="3"/>
+      <c r="K16" s="9">
+        <f t="shared" si="4"/>
         <v>57.692307692307693</v>
       </c>
     </row>

</xml_diff>